<commit_message>
Add score calculations for mastermind
</commit_message>
<xml_diff>
--- a/score_calculations.xlsx
+++ b/score_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\buk-universal-games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33FE437B-DA60-41EC-889F-5C7E829431F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A43C537-5488-414C-888D-52AD07CB06C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15945" windowWidth="25260" windowHeight="15735" xr2:uid="{043E7AFB-4D1A-4CE3-9017-69C2EFF82B06}"/>
+    <workbookView xWindow="62670" yWindow="0" windowWidth="25260" windowHeight="31785" xr2:uid="{043E7AFB-4D1A-4CE3-9017-69C2EFF82B06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="71">
   <si>
     <t>Total 'henge-tid' (T)</t>
   </si>
@@ -219,6 +219,36 @@
   </si>
   <si>
     <t>Calculated values</t>
+  </si>
+  <si>
+    <t>points</t>
+  </si>
+  <si>
+    <t>color_points</t>
+  </si>
+  <si>
+    <t>turn_points</t>
+  </si>
+  <si>
+    <t>correct_colors</t>
+  </si>
+  <si>
+    <t>turns_taken</t>
+  </si>
+  <si>
+    <t>code_guessed_correctly</t>
+  </si>
+  <si>
+    <t>max_turns</t>
+  </si>
+  <si>
+    <t>bottom_score</t>
+  </si>
+  <si>
+    <t>top_score</t>
+  </si>
+  <si>
+    <t>Mastermind</t>
   </si>
 </sst>
 </file>
@@ -226,8 +256,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="169" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    <numFmt numFmtId="175" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -274,14 +304,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -618,25 +647,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB724AC0-3929-4A76-9C7A-4EE51FC73C9A}">
-  <dimension ref="A1:H98"/>
+  <dimension ref="A1:H129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G79" sqref="G79"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>22</v>
       </c>
     </row>
@@ -689,7 +719,7 @@
       <c r="A8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8">
         <v>1</v>
       </c>
     </row>
@@ -697,7 +727,7 @@
       <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9">
         <v>20</v>
       </c>
     </row>
@@ -756,11 +786,11 @@
       <c r="A18" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B18" s="5">
         <f>MEDIAN(0, (B17 - B4) * 20 / (B5 - B4), 20)</f>
         <v>1.9333333333333329</v>
       </c>
-      <c r="C18" s="6"/>
+      <c r="C18" s="5"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
@@ -795,19 +825,19 @@
         <v>0</v>
       </c>
       <c r="C22" s="3">
-        <f>B22*$B$3</f>
+        <f t="shared" ref="C22:C29" si="0">B22*$B$3</f>
         <v>0</v>
       </c>
       <c r="D22" s="3">
         <f>A22-C22</f>
         <v>0</v>
       </c>
-      <c r="E22" s="5">
-        <f>(((D22-$B$4)*($B$9-$B$8))/($B$5-$B$4))+$B$8</f>
+      <c r="E22">
+        <f t="shared" ref="E22:E29" si="1">(((D22-$B$4)*($B$9-$B$8))/($B$5-$B$4))+$B$8</f>
         <v>-6.6000000000000005</v>
       </c>
       <c r="F22" s="2">
-        <f>MEDIAN($B$8, E22, $B$9)</f>
+        <f t="shared" ref="F22:F29" si="2">MEDIAN($B$8, E22, $B$9)</f>
         <v>1</v>
       </c>
     </row>
@@ -819,19 +849,19 @@
         <v>0</v>
       </c>
       <c r="C23" s="3">
-        <f>B23*$B$3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D23" s="3">
-        <f t="shared" ref="D23:D29" si="0">A23-C23</f>
+        <f t="shared" ref="D23:D29" si="3">A23-C23</f>
         <v>1.3888888888888889E-3</v>
       </c>
-      <c r="E23" s="5">
-        <f>(((D23-$B$4)*($B$9-$B$8))/($B$5-$B$4))+$B$8</f>
+      <c r="E23">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="F23" s="2">
-        <f>MEDIAN($B$8, E23, $B$9)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -843,19 +873,19 @@
         <v>0</v>
       </c>
       <c r="C24" s="3">
-        <f>B24*$B$3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D24" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3.472222222222222E-3</v>
       </c>
-      <c r="E24" s="5">
-        <f>(((D24-$B$4)*($B$9-$B$8))/($B$5-$B$4))+$B$8</f>
+      <c r="E24">
+        <f t="shared" si="1"/>
         <v>12.399999999999999</v>
       </c>
       <c r="F24" s="2">
-        <f>MEDIAN($B$8, E24, $B$9)</f>
+        <f t="shared" si="2"/>
         <v>12.399999999999999</v>
       </c>
     </row>
@@ -867,19 +897,19 @@
         <v>0</v>
       </c>
       <c r="C25" s="3">
-        <f>B25*$B$3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D25" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>4.8611111111111112E-3</v>
       </c>
-      <c r="E25" s="5">
-        <f>(((D25-$B$4)*($B$9-$B$8))/($B$5-$B$4))+$B$8</f>
+      <c r="E25">
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="F25" s="2">
-        <f>MEDIAN($B$8, E25, $B$9)</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
     </row>
@@ -891,19 +921,19 @@
         <v>0</v>
       </c>
       <c r="C26" s="3">
-        <f>B26*$B$3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D26" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="E26" s="5">
-        <f>(((D26-$B$4)*($B$9-$B$8))/($B$5-$B$4))+$B$8</f>
+      <c r="E26">
+        <f t="shared" si="1"/>
         <v>31.4</v>
       </c>
       <c r="F26" s="2">
-        <f>MEDIAN($B$8, E26, $B$9)</f>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
     </row>
@@ -915,19 +945,19 @@
         <v>5</v>
       </c>
       <c r="C27" s="3">
-        <f>B27*$B$3</f>
+        <f t="shared" si="0"/>
         <v>5.7870370370370367E-4</v>
       </c>
       <c r="D27" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>8.1018518518518527E-4</v>
       </c>
-      <c r="E27" s="5">
-        <f>(((D27-$B$4)*($B$9-$B$8))/($B$5-$B$4))+$B$8</f>
+      <c r="E27">
+        <f t="shared" si="1"/>
         <v>-2.166666666666667</v>
       </c>
       <c r="F27" s="2">
-        <f>MEDIAN($B$8, E27, $B$9)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -939,19 +969,19 @@
         <v>7</v>
       </c>
       <c r="C28" s="3">
-        <f>B28*$B$3</f>
+        <f t="shared" si="0"/>
         <v>8.1018518518518527E-4</v>
       </c>
       <c r="D28" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.6620370370370365E-3</v>
       </c>
-      <c r="E28" s="5">
-        <f>(((D28-$B$4)*($B$9-$B$8))/($B$5-$B$4))+$B$8</f>
+      <c r="E28">
+        <f t="shared" si="1"/>
         <v>7.9666666666666632</v>
       </c>
       <c r="F28" s="2">
-        <f>MEDIAN($B$8, E28, $B$9)</f>
+        <f t="shared" si="2"/>
         <v>7.9666666666666632</v>
       </c>
     </row>
@@ -963,24 +993,24 @@
         <v>30</v>
       </c>
       <c r="C29" s="3">
-        <f>B29*$B$3</f>
+        <f t="shared" si="0"/>
         <v>3.4722222222222225E-3</v>
       </c>
       <c r="D29" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>3.4722222222222216E-3</v>
       </c>
-      <c r="E29" s="5">
-        <f>(((D29-$B$4)*($B$9-$B$8))/($B$5-$B$4))+$B$8</f>
+      <c r="E29">
+        <f t="shared" si="1"/>
         <v>12.399999999999999</v>
       </c>
       <c r="F29" s="2">
-        <f>MEDIAN($B$8, E29, $B$9)</f>
+        <f t="shared" si="2"/>
         <v>12.399999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="6" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1068,11 +1098,11 @@
       <c r="B44">
         <v>0</v>
       </c>
-      <c r="C44" s="8">
+      <c r="C44" s="7">
         <f>$B$33+(A44-$B$35)*($B$34-$B$33)/($B$36-$B$35)</f>
         <v>1</v>
       </c>
-      <c r="D44" s="8">
+      <c r="D44" s="7">
         <f>$B$33+(B44-$B$35)*($B$34-$B$33)/($B$36-$B$35)</f>
         <v>1</v>
       </c>
@@ -1084,12 +1114,12 @@
       <c r="B45">
         <v>0</v>
       </c>
-      <c r="C45" s="8">
-        <f t="shared" ref="C45:C48" si="1">$B$33+(A45-$B$35)*($B$34-$B$33)/($B$36-$B$35)</f>
+      <c r="C45" s="7">
+        <f t="shared" ref="C45:C48" si="4">$B$33+(A45-$B$35)*($B$34-$B$33)/($B$36-$B$35)</f>
         <v>20</v>
       </c>
-      <c r="D45" s="8">
-        <f t="shared" ref="D45:D48" si="2">$B$33+(B45-$B$35)*($B$34-$B$33)/($B$36-$B$35)</f>
+      <c r="D45" s="7">
+        <f t="shared" ref="D45:D48" si="5">$B$33+(B45-$B$35)*($B$34-$B$33)/($B$36-$B$35)</f>
         <v>1</v>
       </c>
     </row>
@@ -1100,12 +1130,12 @@
       <c r="B46">
         <v>5</v>
       </c>
-      <c r="C46" s="8">
-        <f t="shared" si="1"/>
+      <c r="C46" s="7">
+        <f t="shared" si="4"/>
         <v>11.555555555555555</v>
       </c>
-      <c r="D46" s="8">
-        <f t="shared" si="2"/>
+      <c r="D46" s="7">
+        <f t="shared" si="5"/>
         <v>11.555555555555555</v>
       </c>
     </row>
@@ -1116,12 +1146,12 @@
       <c r="B47">
         <v>7</v>
       </c>
-      <c r="C47" s="8">
-        <f t="shared" si="1"/>
+      <c r="C47" s="7">
+        <f t="shared" si="4"/>
         <v>5.2222222222222223</v>
       </c>
-      <c r="D47" s="8">
-        <f t="shared" si="2"/>
+      <c r="D47" s="7">
+        <f t="shared" si="5"/>
         <v>15.777777777777779</v>
       </c>
     </row>
@@ -1132,17 +1162,17 @@
       <c r="B48">
         <v>9</v>
       </c>
-      <c r="C48" s="8">
-        <f t="shared" si="1"/>
+      <c r="C48" s="7">
+        <f t="shared" si="4"/>
         <v>20</v>
       </c>
-      <c r="D48" s="8">
-        <f t="shared" si="2"/>
+      <c r="D48" s="7">
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
+      <c r="A50" s="6" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1187,7 +1217,7 @@
       <c r="A56" t="s">
         <v>43</v>
       </c>
-      <c r="B56" s="5">
+      <c r="B56">
         <v>4</v>
       </c>
     </row>
@@ -1195,7 +1225,7 @@
       <c r="A57" t="s">
         <v>44</v>
       </c>
-      <c r="B57" s="5">
+      <c r="B57">
         <v>2</v>
       </c>
     </row>
@@ -1203,7 +1233,7 @@
       <c r="A58" t="s">
         <v>45</v>
       </c>
-      <c r="B58" s="5">
+      <c r="B58">
         <v>3</v>
       </c>
     </row>
@@ -1272,7 +1302,7 @@
         <v>0</v>
       </c>
       <c r="C67" s="1"/>
-      <c r="D67" s="8">
+      <c r="D67" s="7">
         <f>IF(A67,$B$58,B67)</f>
         <v>0</v>
       </c>
@@ -1301,24 +1331,24 @@
         <v>2</v>
       </c>
       <c r="C68" s="1"/>
-      <c r="D68" s="8">
-        <f t="shared" ref="D68:D71" si="3">IF(A68,$B$58,B68)</f>
+      <c r="D68" s="7">
+        <f t="shared" ref="D68:D71" si="6">IF(A68,$B$58,B68)</f>
         <v>2</v>
       </c>
       <c r="E68">
-        <f t="shared" ref="E68:E71" si="4">IF(A68,$B$56,0)</f>
+        <f t="shared" ref="E68:E71" si="7">IF(A68,$B$56,0)</f>
         <v>0</v>
       </c>
       <c r="F68" s="1">
-        <f t="shared" ref="F68:F71" si="5">IF(A68,C68,$B$54)</f>
+        <f t="shared" ref="F68:F71" si="8">IF(A68,C68,$B$54)</f>
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="G68">
-        <f t="shared" ref="G68:G71" si="6">$B$53+($B$55-F68)*($B$52-$B$53)/($B$55-$B$54)</f>
+        <f t="shared" ref="G68:G71" si="9">$B$53+($B$55-F68)*($B$52-$B$53)/($B$55-$B$54)</f>
         <v>0</v>
       </c>
       <c r="H68">
-        <f t="shared" ref="H68:H71" si="7">D68*$B$57+E68+G68</f>
+        <f t="shared" ref="H68:H71" si="10">D68*$B$57+E68+G68</f>
         <v>4</v>
       </c>
     </row>
@@ -1329,24 +1359,24 @@
       <c r="C69" s="1">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="D69" s="8">
-        <f t="shared" si="3"/>
+      <c r="D69" s="7">
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="E69">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="F69" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>6.9444444444444441E-3</v>
       </c>
       <c r="G69">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="H69">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
     </row>
@@ -1357,24 +1387,24 @@
       <c r="C70" s="1">
         <v>4.1666666666666666E-3</v>
       </c>
-      <c r="D70" s="8">
-        <f t="shared" si="3"/>
+      <c r="D70" s="7">
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="E70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="F70" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>4.1666666666666666E-3</v>
       </c>
       <c r="G70">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="H70">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>15</v>
       </c>
     </row>
@@ -1385,29 +1415,29 @@
       <c r="C71" s="1">
         <v>1.3888888888888889E-3</v>
       </c>
-      <c r="D71" s="8">
-        <f t="shared" si="3"/>
+      <c r="D71" s="7">
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="E71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>4</v>
       </c>
       <c r="F71" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>1.3888888888888889E-3</v>
       </c>
       <c r="G71">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
       <c r="H71">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>20</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="7" t="s">
+      <c r="A73" s="6" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1452,7 +1482,7 @@
       <c r="A79" t="s">
         <v>48</v>
       </c>
-      <c r="B79" s="5">
+      <c r="B79">
         <v>3</v>
       </c>
     </row>
@@ -1460,7 +1490,7 @@
       <c r="A80" t="s">
         <v>49</v>
       </c>
-      <c r="B80" s="5">
+      <c r="B80">
         <v>0.5</v>
       </c>
     </row>
@@ -1468,7 +1498,7 @@
       <c r="A81" t="s">
         <v>50</v>
       </c>
-      <c r="B81" s="5">
+      <c r="B81">
         <v>0</v>
       </c>
     </row>
@@ -1476,7 +1506,7 @@
       <c r="A82" t="s">
         <v>51</v>
       </c>
-      <c r="B82" s="5">
+      <c r="B82">
         <v>20</v>
       </c>
     </row>
@@ -1505,7 +1535,7 @@
       <c r="A87" t="s">
         <v>54</v>
       </c>
-      <c r="B87" s="5">
+      <c r="B87">
         <v>18</v>
       </c>
     </row>
@@ -1513,7 +1543,7 @@
       <c r="A88" t="s">
         <v>55</v>
       </c>
-      <c r="B88" s="5">
+      <c r="B88">
         <v>5</v>
       </c>
     </row>
@@ -1547,28 +1577,307 @@
         <v>58</v>
       </c>
       <c r="C94" s="1"/>
-      <c r="D94" s="8"/>
+      <c r="D94" s="7"/>
       <c r="F94" s="1"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C95" s="1"/>
-      <c r="D95" s="8"/>
+      <c r="D95" s="7"/>
       <c r="F95" s="1"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C96" s="1"/>
-      <c r="D96" s="8"/>
       <c r="F96" s="1"/>
     </row>
-    <row r="97" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C97" s="1"/>
-      <c r="D97" s="8"/>
-      <c r="F97" s="1"/>
-    </row>
-    <row r="98" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C98" s="1"/>
-      <c r="D98" s="8"/>
-      <c r="F98" s="1"/>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C105" s="1"/>
+      <c r="D105" s="7"/>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>69</v>
+      </c>
+      <c r="B107">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>68</v>
+      </c>
+      <c r="B108">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>67</v>
+      </c>
+      <c r="B109">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>34</v>
+      </c>
+      <c r="B110" s="3">
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>66</v>
+      </c>
+      <c r="B113" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>65</v>
+      </c>
+      <c r="B114">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
+        <v>65</v>
+      </c>
+      <c r="B117" t="s">
+        <v>64</v>
+      </c>
+      <c r="C117" t="s">
+        <v>63</v>
+      </c>
+      <c r="D117" t="s">
+        <v>62</v>
+      </c>
+      <c r="E117" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A118">
+        <v>1</v>
+      </c>
+      <c r="C118">
+        <f>IF(ISBLANK(A118),0,$B$108+(($B$109-A118)/($B$109-1))*($B$107-$B$108))</f>
+        <v>20</v>
+      </c>
+      <c r="D118">
+        <f>B118</f>
+        <v>0</v>
+      </c>
+      <c r="E118">
+        <f>D118+C118</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A119">
+        <v>2</v>
+      </c>
+      <c r="C119">
+        <f>IF(ISBLANK(A119),0,$B$108+(($B$109-A119)/($B$109-1))*($B$107-$B$108))</f>
+        <v>18</v>
+      </c>
+      <c r="D119">
+        <f>B119</f>
+        <v>0</v>
+      </c>
+      <c r="E119">
+        <f>D119+C119</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A120">
+        <v>3</v>
+      </c>
+      <c r="C120">
+        <f>IF(ISBLANK(A120),0,$B$108+(($B$109-A120)/($B$109-1))*($B$107-$B$108))</f>
+        <v>16</v>
+      </c>
+      <c r="D120">
+        <f>B120</f>
+        <v>0</v>
+      </c>
+      <c r="E120">
+        <f>D120+C120</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A121">
+        <v>4</v>
+      </c>
+      <c r="C121">
+        <f>IF(ISBLANK(A121),0,$B$108+(($B$109-A121)/($B$109-1))*($B$107-$B$108))</f>
+        <v>14</v>
+      </c>
+      <c r="D121">
+        <f>B121</f>
+        <v>0</v>
+      </c>
+      <c r="E121">
+        <f>D121+C121</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A122">
+        <v>5</v>
+      </c>
+      <c r="C122">
+        <f>IF(ISBLANK(A122),0,$B$108+(($B$109-A122)/($B$109-1))*($B$107-$B$108))</f>
+        <v>12</v>
+      </c>
+      <c r="D122">
+        <f>B122</f>
+        <v>0</v>
+      </c>
+      <c r="E122">
+        <f>D122+C122</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A123">
+        <v>6</v>
+      </c>
+      <c r="C123">
+        <f>IF(ISBLANK(A123),0,$B$108+(($B$109-A123)/($B$109-1))*($B$107-$B$108))</f>
+        <v>10</v>
+      </c>
+      <c r="D123">
+        <f>B123</f>
+        <v>0</v>
+      </c>
+      <c r="E123">
+        <f>D123+C123</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A124">
+        <v>7</v>
+      </c>
+      <c r="C124">
+        <f>IF(ISBLANK(A124),0,$B$108+(($B$109-A124)/($B$109-1))*($B$107-$B$108))</f>
+        <v>8</v>
+      </c>
+      <c r="D124">
+        <f>B124</f>
+        <v>0</v>
+      </c>
+      <c r="E124">
+        <f>D124+C124</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125">
+        <v>8</v>
+      </c>
+      <c r="C125">
+        <f>IF(ISBLANK(A125),0,$B$108+(($B$109-A125)/($B$109-1))*($B$107-$B$108))</f>
+        <v>6</v>
+      </c>
+      <c r="D125">
+        <f>B125</f>
+        <v>0</v>
+      </c>
+      <c r="E125">
+        <f>D125+C125</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B126">
+        <v>4</v>
+      </c>
+      <c r="C126">
+        <f>IF(ISBLANK(A126),0,$B$108+(($B$109-A126)/($B$109-1))*($B$107-$B$108))</f>
+        <v>0</v>
+      </c>
+      <c r="D126">
+        <f>B126</f>
+        <v>4</v>
+      </c>
+      <c r="E126">
+        <f>D126+C126</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B127">
+        <v>3</v>
+      </c>
+      <c r="C127">
+        <f>IF(ISBLANK(A127),0,$B$108+(($B$109-A127)/($B$109-1))*($B$107-$B$108))</f>
+        <v>0</v>
+      </c>
+      <c r="D127">
+        <f>B127</f>
+        <v>3</v>
+      </c>
+      <c r="E127">
+        <f>D127+C127</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B128">
+        <v>2</v>
+      </c>
+      <c r="C128">
+        <f>IF(ISBLANK(A128),0,$B$108+(($B$109-A128)/($B$109-1))*($B$107-$B$108))</f>
+        <v>0</v>
+      </c>
+      <c r="D128">
+        <f>B128</f>
+        <v>2</v>
+      </c>
+      <c r="E128">
+        <f>D128+C128</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B129">
+        <v>1</v>
+      </c>
+      <c r="C129">
+        <f>IF(ISBLANK(A129),0,$B$108+(($B$109-A129)/($B$109-1))*($B$107-$B$108))</f>
+        <v>0</v>
+      </c>
+      <c r="D129">
+        <f>B129</f>
+        <v>1</v>
+      </c>
+      <c r="E129">
+        <f>D129+C129</f>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finish score calculation for hamster wheel. All score calculations are finished.
</commit_message>
<xml_diff>
--- a/score_calculations.xlsx
+++ b/score_calculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\buk-universal-games\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A43C537-5488-414C-888D-52AD07CB06C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36719912-9B9B-4979-B5D4-A42918B4E0B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="62670" yWindow="0" windowWidth="25260" windowHeight="31785" xr2:uid="{043E7AFB-4D1A-4CE3-9017-69C2EFF82B06}"/>
+    <workbookView xWindow="86400" yWindow="105" windowWidth="28800" windowHeight="31575" xr2:uid="{043E7AFB-4D1A-4CE3-9017-69C2EFF82B06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="71">
   <si>
     <t>Total 'henge-tid' (T)</t>
   </si>
@@ -194,27 +194,9 @@
     <t>max_step_penalties</t>
   </si>
   <si>
-    <t>time_team1</t>
-  </si>
-  <si>
-    <t>time_team2</t>
-  </si>
-  <si>
-    <t>steps_outside_team1</t>
-  </si>
-  <si>
-    <t>steps_outside_team2</t>
-  </si>
-  <si>
     <t>winner</t>
   </si>
   <si>
-    <t>team1</t>
-  </si>
-  <si>
-    <t>team2</t>
-  </si>
-  <si>
     <t>clamp step count</t>
   </si>
   <si>
@@ -249,6 +231,24 @@
   </si>
   <si>
     <t>Mastermind</t>
+  </si>
+  <si>
+    <t>time points</t>
+  </si>
+  <si>
+    <t>penalty points</t>
+  </si>
+  <si>
+    <t>total points</t>
+  </si>
+  <si>
+    <t>team</t>
+  </si>
+  <si>
+    <t>max penalty:</t>
+  </si>
+  <si>
+    <t>steps outside</t>
   </si>
 </sst>
 </file>
@@ -647,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB724AC0-3929-4A76-9C7A-4EE51FC73C9A}">
-  <dimension ref="A1:H129"/>
+  <dimension ref="A1:H124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1451,7 +1451,7 @@
         <v>24</v>
       </c>
       <c r="B75">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -1459,7 +1459,8 @@
         <v>25</v>
       </c>
       <c r="B76">
-        <v>17</v>
+        <f>20-B79</f>
+        <v>15</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -1483,7 +1484,7 @@
         <v>48</v>
       </c>
       <c r="B79">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -1491,10 +1492,10 @@
         <v>49</v>
       </c>
       <c r="B80">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>50</v>
       </c>
@@ -1502,186 +1503,384 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>51</v>
       </c>
       <c r="B82">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>69</v>
+      </c>
+      <c r="B84">
+        <f>B82*B80</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>52</v>
+      </c>
+      <c r="B87">
+        <f>IF(B89 &lt; B90, 1, IF(B89 &gt; B90, IF(C90 &lt; C89, 1, 2)))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>68</v>
+      </c>
+      <c r="B88" t="s">
+        <v>38</v>
+      </c>
+      <c r="C88" t="s">
+        <v>70</v>
+      </c>
+      <c r="D88" t="s">
+        <v>53</v>
+      </c>
+      <c r="E88" t="s">
+        <v>65</v>
+      </c>
+      <c r="F88" t="s">
+        <v>66</v>
+      </c>
+      <c r="G88" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>1</v>
+      </c>
+      <c r="B89" s="3">
+        <v>1.261574074074074E-3</v>
+      </c>
+      <c r="C89">
+        <v>18</v>
+      </c>
+      <c r="D89">
+        <f>MEDIAN($B$81,C89,$B$82)</f>
+        <v>10</v>
+      </c>
+      <c r="E89">
+        <f>$B$76-((B89-$B$77)*($B$76-$B$75))/($B$78-$B$77)</f>
+        <v>11.461111111111112</v>
+      </c>
+      <c r="F89">
+        <f>D89*$B$80</f>
+        <v>2</v>
+      </c>
+      <c r="G89">
+        <f>E89-F89 +IF($B$87=A89,$B$79,0)</f>
+        <v>14.461111111111112</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>2</v>
+      </c>
+      <c r="B90" s="3">
+        <v>1.8518518518518519E-3</v>
+      </c>
+      <c r="C90">
+        <v>5</v>
+      </c>
+      <c r="D90">
+        <f>MEDIAN($B$81,C90,$B$82)</f>
+        <v>5</v>
+      </c>
+      <c r="E90">
+        <f>$B$76-((B90-$B$77)*($B$76-$B$75))/($B$78-$B$77)</f>
+        <v>7.7777777777777777</v>
+      </c>
+      <c r="F90">
+        <f>D90*$B$80</f>
+        <v>1</v>
+      </c>
+      <c r="G90">
+        <f>E90-F90 +IF($B$87=A90,$B$79,0)</f>
+        <v>6.7777777777777777</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C91" s="1"/>
+      <c r="D91" s="7"/>
+      <c r="F91" s="1"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>52</v>
+      </c>
+      <c r="B92">
+        <f>IF(B94 &lt; B95, 1, IF(B94 &gt; B95, IF(C95 &lt; C94, 1, 2)))</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>68</v>
+      </c>
+      <c r="B93" t="s">
+        <v>38</v>
+      </c>
+      <c r="C93" t="s">
+        <v>70</v>
+      </c>
+      <c r="D93" t="s">
+        <v>53</v>
+      </c>
+      <c r="E93" t="s">
+        <v>65</v>
+      </c>
+      <c r="F93" t="s">
+        <v>66</v>
+      </c>
+      <c r="G93" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>1</v>
+      </c>
+      <c r="B94" s="3">
+        <v>3.4722222222222224E-4</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <f>MEDIAN($B$81,C94,$B$82)</f>
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <f>$B$76-((MEDIAN($B$77,B94,$B$78)-$B$77)*($B$76-$B$75))/($B$78-$B$77)</f>
+        <v>15</v>
+      </c>
+      <c r="F94">
+        <f>D94*$B$80</f>
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <f>E94-F94 +IF($B$87=A94,$B$79,0)</f>
         <v>20</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="4" t="s">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>2</v>
+      </c>
+      <c r="B95" s="3">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="C95">
+        <v>100</v>
+      </c>
+      <c r="D95">
+        <f>MEDIAN($B$81,C95,$B$82)</f>
+        <v>10</v>
+      </c>
+      <c r="E95">
+        <f>$B$76-((MEDIAN($B$77,B95,$B$78)-$B$77)*($B$76-$B$75))/($B$78-$B$77)</f>
+        <v>2</v>
+      </c>
+      <c r="F95">
+        <f>D95*$B$80</f>
+        <v>2</v>
+      </c>
+      <c r="G95">
+        <f>E95-F95 +IF($B$87=A95,$B$79,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C100" s="1"/>
+      <c r="D100" s="7"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>63</v>
+      </c>
+      <c r="B102">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>62</v>
+      </c>
+      <c r="B103">
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>52</v>
-      </c>
-      <c r="B85" s="3">
-        <v>1.261574074074074E-3</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>53</v>
-      </c>
-      <c r="B86" s="3">
-        <v>1.8518518518518519E-3</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>54</v>
-      </c>
-      <c r="B87">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>61</v>
+      </c>
+      <c r="B104">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>34</v>
+      </c>
+      <c r="B105" s="3">
+        <v>6.9444444444444441E-3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>60</v>
+      </c>
+      <c r="B108" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>59</v>
+      </c>
+      <c r="B109">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>59</v>
+      </c>
+      <c r="B112" t="s">
+        <v>58</v>
+      </c>
+      <c r="C112" t="s">
+        <v>57</v>
+      </c>
+      <c r="D112" t="s">
+        <v>56</v>
+      </c>
+      <c r="E112" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A113">
+        <v>1</v>
+      </c>
+      <c r="C113">
+        <f>IF(ISBLANK(A113),0,$B$103+(($B$104-A113)/($B$104-1))*($B$102-$B$103))</f>
+        <v>20</v>
+      </c>
+      <c r="D113">
+        <f>B113</f>
+        <v>0</v>
+      </c>
+      <c r="E113">
+        <f>D113+C113</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <v>2</v>
+      </c>
+      <c r="C114">
+        <f>IF(ISBLANK(A114),0,$B$103+(($B$104-A114)/($B$104-1))*($B$102-$B$103))</f>
         <v>18</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>55</v>
-      </c>
-      <c r="B88">
+      <c r="D114">
+        <f>B114</f>
+        <v>0</v>
+      </c>
+      <c r="E114">
+        <f>D114+C114</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <v>3</v>
+      </c>
+      <c r="C115">
+        <f>IF(ISBLANK(A115),0,$B$103+(($B$104-A115)/($B$104-1))*($B$102-$B$103))</f>
+        <v>16</v>
+      </c>
+      <c r="D115">
+        <f>B115</f>
+        <v>0</v>
+      </c>
+      <c r="E115">
+        <f>D115+C115</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <v>4</v>
+      </c>
+      <c r="C116">
+        <f>IF(ISBLANK(A116),0,$B$103+(($B$104-A116)/($B$104-1))*($B$102-$B$103))</f>
+        <v>14</v>
+      </c>
+      <c r="D116">
+        <f>B116</f>
+        <v>0</v>
+      </c>
+      <c r="E116">
+        <f>D116+C116</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A117">
         <v>5</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>56</v>
-      </c>
-      <c r="B91">
-        <f>IF(B85 &lt; B86, 1, IF(B85 &gt; B86, IF(B88 &lt; B87, 1, 2)))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="4"/>
-      <c r="B92" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>58</v>
-      </c>
-      <c r="C94" s="1"/>
-      <c r="D94" s="7"/>
-      <c r="F94" s="1"/>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C95" s="1"/>
-      <c r="D95" s="7"/>
-      <c r="F95" s="1"/>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F96" s="1"/>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A105" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C105" s="1"/>
-      <c r="D105" s="7"/>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>69</v>
-      </c>
-      <c r="B107">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>68</v>
-      </c>
-      <c r="B108">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
-        <v>67</v>
-      </c>
-      <c r="B109">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
-        <v>34</v>
-      </c>
-      <c r="B110" s="3">
-        <v>6.9444444444444441E-3</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>66</v>
-      </c>
-      <c r="B113" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>65</v>
-      </c>
-      <c r="B114">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>65</v>
-      </c>
-      <c r="B117" t="s">
-        <v>64</v>
-      </c>
-      <c r="C117" t="s">
-        <v>63</v>
-      </c>
-      <c r="D117" t="s">
-        <v>62</v>
-      </c>
-      <c r="E117" t="s">
-        <v>61</v>
+      <c r="C117">
+        <f>IF(ISBLANK(A117),0,$B$103+(($B$104-A117)/($B$104-1))*($B$102-$B$103))</f>
+        <v>12</v>
+      </c>
+      <c r="D117">
+        <f>B117</f>
+        <v>0</v>
+      </c>
+      <c r="E117">
+        <f>D117+C117</f>
+        <v>12</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C118">
-        <f>IF(ISBLANK(A118),0,$B$108+(($B$109-A118)/($B$109-1))*($B$107-$B$108))</f>
-        <v>20</v>
+        <f>IF(ISBLANK(A118),0,$B$103+(($B$104-A118)/($B$104-1))*($B$102-$B$103))</f>
+        <v>10</v>
       </c>
       <c r="D118">
         <f>B118</f>
@@ -1689,16 +1888,16 @@
       </c>
       <c r="E118">
         <f>D118+C118</f>
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C119">
-        <f>IF(ISBLANK(A119),0,$B$108+(($B$109-A119)/($B$109-1))*($B$107-$B$108))</f>
-        <v>18</v>
+        <f>IF(ISBLANK(A119),0,$B$103+(($B$104-A119)/($B$104-1))*($B$102-$B$103))</f>
+        <v>8</v>
       </c>
       <c r="D119">
         <f>B119</f>
@@ -1706,16 +1905,16 @@
       </c>
       <c r="E119">
         <f>D119+C119</f>
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C120">
-        <f>IF(ISBLANK(A120),0,$B$108+(($B$109-A120)/($B$109-1))*($B$107-$B$108))</f>
-        <v>16</v>
+        <f>IF(ISBLANK(A120),0,$B$103+(($B$104-A120)/($B$104-1))*($B$102-$B$103))</f>
+        <v>6</v>
       </c>
       <c r="D120">
         <f>B120</f>
@@ -1723,159 +1922,74 @@
       </c>
       <c r="E120">
         <f>D120+C120</f>
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A121">
+      <c r="B121">
         <v>4</v>
       </c>
       <c r="C121">
-        <f>IF(ISBLANK(A121),0,$B$108+(($B$109-A121)/($B$109-1))*($B$107-$B$108))</f>
-        <v>14</v>
+        <f>IF(ISBLANK(A121),0,$B$103+(($B$104-A121)/($B$104-1))*($B$102-$B$103))</f>
+        <v>0</v>
       </c>
       <c r="D121">
         <f>B121</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E121">
         <f>D121+C121</f>
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A122">
-        <v>5</v>
+      <c r="B122">
+        <v>3</v>
       </c>
       <c r="C122">
-        <f>IF(ISBLANK(A122),0,$B$108+(($B$109-A122)/($B$109-1))*($B$107-$B$108))</f>
-        <v>12</v>
+        <f>IF(ISBLANK(A122),0,$B$103+(($B$104-A122)/($B$104-1))*($B$102-$B$103))</f>
+        <v>0</v>
       </c>
       <c r="D122">
         <f>B122</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E122">
         <f>D122+C122</f>
-        <v>12</v>
+        <v>3</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A123">
-        <v>6</v>
+      <c r="B123">
+        <v>2</v>
       </c>
       <c r="C123">
-        <f>IF(ISBLANK(A123),0,$B$108+(($B$109-A123)/($B$109-1))*($B$107-$B$108))</f>
-        <v>10</v>
+        <f>IF(ISBLANK(A123),0,$B$103+(($B$104-A123)/($B$104-1))*($B$102-$B$103))</f>
+        <v>0</v>
       </c>
       <c r="D123">
         <f>B123</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E123">
         <f>D123+C123</f>
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124">
-        <v>7</v>
+      <c r="B124">
+        <v>1</v>
       </c>
       <c r="C124">
-        <f>IF(ISBLANK(A124),0,$B$108+(($B$109-A124)/($B$109-1))*($B$107-$B$108))</f>
-        <v>8</v>
+        <f>IF(ISBLANK(A124),0,$B$103+(($B$104-A124)/($B$104-1))*($B$102-$B$103))</f>
+        <v>0</v>
       </c>
       <c r="D124">
         <f>B124</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E124">
         <f>D124+C124</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A125">
-        <v>8</v>
-      </c>
-      <c r="C125">
-        <f>IF(ISBLANK(A125),0,$B$108+(($B$109-A125)/($B$109-1))*($B$107-$B$108))</f>
-        <v>6</v>
-      </c>
-      <c r="D125">
-        <f>B125</f>
-        <v>0</v>
-      </c>
-      <c r="E125">
-        <f>D125+C125</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B126">
-        <v>4</v>
-      </c>
-      <c r="C126">
-        <f>IF(ISBLANK(A126),0,$B$108+(($B$109-A126)/($B$109-1))*($B$107-$B$108))</f>
-        <v>0</v>
-      </c>
-      <c r="D126">
-        <f>B126</f>
-        <v>4</v>
-      </c>
-      <c r="E126">
-        <f>D126+C126</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B127">
-        <v>3</v>
-      </c>
-      <c r="C127">
-        <f>IF(ISBLANK(A127),0,$B$108+(($B$109-A127)/($B$109-1))*($B$107-$B$108))</f>
-        <v>0</v>
-      </c>
-      <c r="D127">
-        <f>B127</f>
-        <v>3</v>
-      </c>
-      <c r="E127">
-        <f>D127+C127</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B128">
-        <v>2</v>
-      </c>
-      <c r="C128">
-        <f>IF(ISBLANK(A128),0,$B$108+(($B$109-A128)/($B$109-1))*($B$107-$B$108))</f>
-        <v>0</v>
-      </c>
-      <c r="D128">
-        <f>B128</f>
-        <v>2</v>
-      </c>
-      <c r="E128">
-        <f>D128+C128</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="129" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B129">
-        <v>1</v>
-      </c>
-      <c r="C129">
-        <f>IF(ISBLANK(A129),0,$B$108+(($B$109-A129)/($B$109-1))*($B$107-$B$108))</f>
-        <v>0</v>
-      </c>
-      <c r="D129">
-        <f>B129</f>
-        <v>1</v>
-      </c>
-      <c r="E129">
-        <f>D129+C129</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>